<commit_message>
get long and lat 2
</commit_message>
<xml_diff>
--- a/extract_features_from_data/address2.xlsx
+++ b/extract_features_from_data/address2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/48ba43577289859f/Documents/code/HCMUS/IntroduceDS/intro-to-ds-project/extract_features_from_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9044A93F-8B7D-4ED9-AB54-E039F9FA4836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{29B3E136-A5EE-4CBD-8AFA-EE781CBC305C}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9044A93F-8B7D-4ED9-AB54-E039F9FA4836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF2784F9-943E-4EE6-97CE-E12A678988B6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9596" uniqueCount="6319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9610" uniqueCount="6331">
   <si>
     <t>Address2</t>
   </si>
@@ -18977,13 +18977,49 @@
   </si>
   <si>
     <t>1.067.186.909</t>
+  </si>
+  <si>
+    <t>10.810.156</t>
+  </si>
+  <si>
+    <t>106.689.889</t>
+  </si>
+  <si>
+    <t>20.848.079</t>
+  </si>
+  <si>
+    <t>106.664.707</t>
+  </si>
+  <si>
+    <t>10.731.584</t>
+  </si>
+  <si>
+    <t>106.687.438</t>
+  </si>
+  <si>
+    <t>10.814.352</t>
+  </si>
+  <si>
+    <t>106.729.918</t>
+  </si>
+  <si>
+    <t>10.759.295</t>
+  </si>
+  <si>
+    <t>106.684.096</t>
+  </si>
+  <si>
+    <t>10.803.420</t>
+  </si>
+  <si>
+    <t>106.689.692</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -19019,6 +19055,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -19099,7 +19141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -19131,6 +19173,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -19146,6 +19191,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19435,8 +19484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3002" workbookViewId="0">
-      <selection activeCell="D3008" sqref="D3008"/>
+    <sheetView tabSelected="1" topLeftCell="A3004" workbookViewId="0">
+      <selection activeCell="E3012" sqref="E3012"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -60693,60 +60742,102 @@
         <v>6216</v>
       </c>
     </row>
-    <row r="3008" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3008" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3008" s="1">
         <v>3006</v>
       </c>
       <c r="B3008" t="s">
         <v>1394</v>
       </c>
-    </row>
-    <row r="3009" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3008" s="11" t="s">
+        <v>6319</v>
+      </c>
+      <c r="D3008" s="11" t="s">
+        <v>6320</v>
+      </c>
+    </row>
+    <row r="3009" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3009" s="1">
         <v>3007</v>
       </c>
       <c r="B3009" t="s">
         <v>2605</v>
       </c>
-    </row>
-    <row r="3010" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3009" s="11" t="s">
+        <v>6321</v>
+      </c>
+      <c r="D3009" s="11" t="s">
+        <v>6322</v>
+      </c>
+    </row>
+    <row r="3010" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3010" s="1">
         <v>3008</v>
       </c>
       <c r="B3010" t="s">
         <v>2606</v>
       </c>
-    </row>
-    <row r="3011" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3010" s="11" t="s">
+        <v>6323</v>
+      </c>
+      <c r="D3010" s="11" t="s">
+        <v>6324</v>
+      </c>
+    </row>
+    <row r="3011" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3011" s="1">
         <v>3009</v>
       </c>
       <c r="B3011" t="s">
         <v>2607</v>
       </c>
-    </row>
-    <row r="3012" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3011" s="11" t="s">
+        <v>6325</v>
+      </c>
+      <c r="D3011" s="11" t="s">
+        <v>6326</v>
+      </c>
+    </row>
+    <row r="3012" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3012" s="1">
         <v>3010</v>
       </c>
       <c r="B3012" t="s">
         <v>2607</v>
       </c>
-    </row>
-    <row r="3013" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3012" s="11" t="s">
+        <v>6325</v>
+      </c>
+      <c r="D3012" s="11" t="s">
+        <v>6326</v>
+      </c>
+    </row>
+    <row r="3013" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3013" s="1">
         <v>3011</v>
       </c>
       <c r="B3013" t="s">
         <v>2462</v>
       </c>
-    </row>
-    <row r="3014" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3013" s="11" t="s">
+        <v>6327</v>
+      </c>
+      <c r="D3013" s="11" t="s">
+        <v>6328</v>
+      </c>
+    </row>
+    <row r="3014" spans="1:4" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3014" s="1">
         <v>3012</v>
       </c>
       <c r="B3014" t="s">
         <v>2608</v>
+      </c>
+      <c r="C3014" s="11" t="s">
+        <v>6329</v>
+      </c>
+      <c r="D3014" s="11" t="s">
+        <v>6330</v>
       </c>
     </row>
     <row r="3015" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>